<commit_message>
confirm changes to 800_reqs
</commit_message>
<xml_diff>
--- a/lib/us_core_test_kit/requirements/hl7.fhir.us.core_8.0.0_reqs.xlsx
+++ b/lib/us_core_test_kit/requirements/hl7.fhir.us.core_8.0.0_reqs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edeyoung/Documents/inferno/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunweiw/github/inferno/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0FAD40-0710-9C4B-87C9-078AF63027A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7023C2-6F1B-564D-85E0-E316D8330894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55860" yWindow="-3520" windowWidth="47500" windowHeight="23100" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19660" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -60,44 +60,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={B414CC66-241E-2941-9511-E5A9A2CC718A}</author>
-    <author>tc={F366D5F7-196A-3845-BEF2-50CD06C3E313}</author>
-    <author>tc={CC199657-803B-CB4B-8A31-16982CABD678}</author>
-  </authors>
-  <commentList>
-    <comment ref="C32" authorId="0" shapeId="0" xr:uid="{B414CC66-241E-2941-9511-E5A9A2CC718A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This is duplicate as line 1. And from the context, this is more like a statement than a requirement.</t>
-      </text>
-    </comment>
-    <comment ref="D261" authorId="1" shapeId="0" xr:uid="{F366D5F7-196A-3845-BEF2-50CD06C3E313}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Searching with encounter is not mandatory. So this should be SHOULD.</t>
-      </text>
-    </comment>
-    <comment ref="D273" authorId="2" shapeId="0" xr:uid="{CC199657-803B-CB4B-8A31-16982CABD678}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Why is this a SHALL requirement? I think it is more like a SHOULD as a recommendation to developers</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -5803,9 +5767,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Yunwei Wang" id="{37F2600B-88C6-1343-8F82-D1B7908C9C14}" userId="S::YUNWEIW@MITRE.ORG::304fa8a3-f6b4-47c4-8daf-6dee396ec296" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6123,20 +6085,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C32" dT="2025-07-03T14:33:51.09" personId="{37F2600B-88C6-1343-8F82-D1B7908C9C14}" id="{B414CC66-241E-2941-9511-E5A9A2CC718A}" done="1">
-    <text>This is duplicate as line 1. And from the context, this is more like a statement than a requirement.</text>
-  </threadedComment>
-  <threadedComment ref="D261" dT="2025-07-03T14:25:59.01" personId="{37F2600B-88C6-1343-8F82-D1B7908C9C14}" id="{F366D5F7-196A-3845-BEF2-50CD06C3E313}" done="1">
-    <text>Searching with encounter is not mandatory. So this should be SHOULD.</text>
-  </threadedComment>
-  <threadedComment ref="D273" dT="2025-07-03T15:39:31.77" personId="{37F2600B-88C6-1343-8F82-D1B7908C9C14}" id="{CC199657-803B-CB4B-8A31-16982CABD678}" done="1">
-    <text>Why is this a SHALL requirement? I think it is more like a SHOULD as a recommendation to developers</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AA7094-ECFF-0B4E-A5C9-6F41B8D76EEB}">
   <dimension ref="A1:C11"/>
@@ -6235,14 +6183,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
   <dimension ref="A1:W655"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="I42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25243,7 +25191,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="470" spans="1:23" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:23" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A470" s="7">
         <v>469</v>
       </c>
@@ -25324,7 +25272,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="472" spans="1:23" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:23" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A472" s="7">
         <v>471</v>
       </c>
@@ -30929,7 +30877,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId14"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -31230,15 +31177,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -31492,6 +31430,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
   <ds:schemaRefs>
@@ -31511,14 +31458,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C0B0A19-6928-4F0B-831A-5B9FDDD3F6CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31536,4 +31475,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
noted 'not tested' for requriements 864 and 866 as these are errors in the specificatio. Regenerated csvs.
</commit_message>
<xml_diff>
--- a/lib/us_core_test_kit/requirements/hl7.fhir.us.core_8.0.0_reqs.xlsx
+++ b/lib/us_core_test_kit/requirements/hl7.fhir.us.core_8.0.0_reqs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edeyoung/Documents/inferno/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5CCC6B-D1B4-F64D-A06A-1F91246BC5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B885EF-E9C6-C248-A89D-DC3149FA7866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50200" yWindow="-5200" windowWidth="40380" windowHeight="18880" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="-57340" yWindow="-6540" windowWidth="40380" windowHeight="28200" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Column Data" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirements!$A$1:$W$656</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirements!$A$1:$X$656</definedName>
     <definedName name="EXPLODE" localSheetId="0">_xlfn.LAMBDA(_xlpm.string,_xlfn.MAKEARRAY(1,LEN(_xlpm.string),_xlfn.LAMBDA(_xlpm.r,_xlpm.c,MID(_xlpm.string,_xlpm.c,1))))</definedName>
     <definedName name="EXPLODE">_xlfn.LAMBDA(_xlpm.string,_xlfn.MAKEARRAY(1,LEN(_xlpm.string),_xlfn.LAMBDA(_xlpm.r,_xlpm.c,MID(_xlpm.string,_xlpm.c,1))))</definedName>
     <definedName name="FIND_DUPLICATES" localSheetId="0">_xlfn.LAMBDA(_xlpm.test_word,_xlpm.test_key,_xlpm.words,_xlpm.keys,_xlpm.threshold, _xlfn.LET(_xlpm.duplist,_xlfn._xlws.FILTER(_xlpm.keys,_xlfn.BYROW(_xlpm.words, _xlfn.LAMBDA(_xlpm.word, Info!HAMDIST(INDEX(_xlpm.word,1,1), _xlpm.test_word)&lt;_xlpm.threshold))),_xlfn.SINGLE(_xlfn._xlws.FILTER(_xlpm.duplist,_xlpm.duplist&lt;&gt;_xlpm.test_key,""))))</definedName>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3569" uniqueCount="1159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3575" uniqueCount="1161">
   <si>
     <r>
       <rPr>
@@ -5163,6 +5163,12 @@
   </si>
   <si>
     <t>validation?</t>
+  </si>
+  <si>
+    <t>This is an error in the specification. See https://jira.hl7.org/browse/FHIR-51493</t>
+  </si>
+  <si>
+    <t>This is a known error in the specification. See https://jira.hl7.org/browse/FHIR-51493</t>
   </si>
 </sst>
 </file>
@@ -6202,10 +6208,10 @@
   <dimension ref="A1:X656"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="V636" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="I592" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X657" sqref="X657"/>
+      <selection pane="bottomRight" activeCell="L657" sqref="L657"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6302,7 +6308,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" s="5" customFormat="1" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -6809,7 +6815,7 @@
       <c r="U11" s="12"/>
       <c r="V11" s="12"/>
     </row>
-    <row r="12" spans="1:23" s="5" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" s="5" customFormat="1" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -6870,7 +6876,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="5" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" s="5" customFormat="1" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -6931,7 +6937,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="5" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" s="5" customFormat="1" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -7023,7 +7029,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -7071,7 +7077,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -7113,7 +7119,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -7155,7 +7161,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -7203,7 +7209,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -7245,7 +7251,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -7287,7 +7293,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -7368,7 +7374,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -7536,7 +7542,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="153" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -7986,7 +7992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -8031,7 +8037,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -8073,7 +8079,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -8115,7 +8121,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -8157,7 +8163,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -8202,7 +8208,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -8244,7 +8250,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -8286,7 +8292,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -8328,7 +8334,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="238" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" ht="238" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -8370,7 +8376,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -8412,7 +8418,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -8493,7 +8499,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -8532,7 +8538,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -8643,7 +8649,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -8754,7 +8760,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -8866,7 +8872,7 @@
       </c>
       <c r="T61" s="12"/>
     </row>
-    <row r="62" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -8905,7 +8911,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -8980,7 +8986,7 @@
         <v>Server</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>64</v>
       </c>
@@ -9061,7 +9067,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -9100,7 +9106,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -9139,7 +9145,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -9178,7 +9184,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -9345,7 +9351,7 @@
       <c r="U73" s="40"/>
       <c r="V73" s="40"/>
     </row>
-    <row r="74" spans="1:23" s="36" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:23" s="36" customFormat="1" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
         <v>73</v>
       </c>
@@ -9396,7 +9402,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="75" spans="1:23" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" s="36" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
         <v>74</v>
       </c>
@@ -9447,7 +9453,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="76" spans="1:23" s="36" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:23" s="36" customFormat="1" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
         <v>75</v>
       </c>
@@ -9580,7 +9586,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
         <v>78</v>
       </c>
@@ -9820,7 +9826,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
         <v>84</v>
       </c>
@@ -9916,7 +9922,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
         <v>86</v>
       </c>
@@ -9958,7 +9964,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
         <v>87</v>
       </c>
@@ -10087,7 +10093,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
         <v>90</v>
       </c>
@@ -10129,7 +10135,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
         <v>91</v>
       </c>
@@ -10204,7 +10210,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
         <v>93</v>
       </c>
@@ -10246,7 +10252,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
         <v>94</v>
       </c>
@@ -10327,7 +10333,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="7">
         <v>96</v>
       </c>
@@ -10369,7 +10375,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
         <v>97</v>
       </c>
@@ -10444,7 +10450,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
         <v>99</v>
       </c>
@@ -10663,7 +10669,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
         <v>105</v>
       </c>
@@ -10812,7 +10818,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
         <v>109</v>
       </c>
@@ -10893,7 +10899,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="272" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:23" ht="272" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
         <v>111</v>
       </c>
@@ -11064,7 +11070,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="7">
         <v>115</v>
       </c>
@@ -11232,7 +11238,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
         <v>119</v>
       </c>
@@ -11277,7 +11283,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="7">
         <v>120</v>
       </c>
@@ -11319,7 +11325,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
         <v>121</v>
       </c>
@@ -11358,7 +11364,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
         <v>122</v>
       </c>
@@ -11397,7 +11403,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
         <v>123</v>
       </c>
@@ -11439,7 +11445,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="7">
         <v>124</v>
       </c>
@@ -11586,7 +11592,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
         <v>128</v>
       </c>
@@ -11664,7 +11670,7 @@
         <v>Server</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
         <v>130</v>
       </c>
@@ -11742,7 +11748,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="153" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:23" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="7">
         <v>132</v>
       </c>
@@ -11790,7 +11796,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="134" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="7">
         <v>133</v>
       </c>
@@ -11835,7 +11841,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="7">
         <v>134</v>
       </c>
@@ -11880,7 +11886,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="136" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="7">
         <v>135</v>
       </c>
@@ -11925,7 +11931,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="137" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="7">
         <v>136</v>
       </c>
@@ -11970,7 +11976,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="138" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="7">
         <v>137</v>
       </c>
@@ -12015,7 +12021,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="139" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="7">
         <v>138</v>
       </c>
@@ -12060,7 +12066,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="140" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="7">
         <v>139</v>
       </c>
@@ -12105,7 +12111,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="141" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="7">
         <v>140</v>
       </c>
@@ -12150,7 +12156,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="142" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="7">
         <v>141</v>
       </c>
@@ -12195,7 +12201,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="143" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="7">
         <v>142</v>
       </c>
@@ -12240,7 +12246,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="144" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="7">
         <v>143</v>
       </c>
@@ -12285,7 +12291,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="145" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="7">
         <v>144</v>
       </c>
@@ -12330,7 +12336,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="146" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="7">
         <v>145</v>
       </c>
@@ -12375,7 +12381,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="147" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="7">
         <v>146</v>
       </c>
@@ -12420,7 +12426,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="7">
         <v>147</v>
       </c>
@@ -12465,7 +12471,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="149" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="7">
         <v>148</v>
       </c>
@@ -12510,7 +12516,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="150" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="7">
         <v>149</v>
       </c>
@@ -12555,7 +12561,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="7">
         <v>150</v>
       </c>
@@ -12600,7 +12606,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="7">
         <v>151</v>
       </c>
@@ -12645,7 +12651,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="7">
         <v>152</v>
       </c>
@@ -12690,7 +12696,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="7">
         <v>153</v>
       </c>
@@ -12735,7 +12741,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="7">
         <v>154</v>
       </c>
@@ -12780,7 +12786,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
         <v>155</v>
       </c>
@@ -12903,7 +12909,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="7">
         <v>158</v>
       </c>
@@ -12945,7 +12951,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="153" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:23" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="7">
         <v>159</v>
       </c>
@@ -12987,7 +12993,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="7">
         <v>160</v>
       </c>
@@ -13029,7 +13035,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="7">
         <v>161</v>
       </c>
@@ -13071,7 +13077,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="153" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:23" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="7">
         <v>162</v>
       </c>
@@ -13113,7 +13119,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="164" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="7">
         <v>163</v>
       </c>
@@ -13155,7 +13161,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="165" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="7">
         <v>164</v>
       </c>
@@ -13197,7 +13203,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="166" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="7">
         <v>165</v>
       </c>
@@ -13281,7 +13287,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="7">
         <v>167</v>
       </c>
@@ -13329,7 +13335,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7">
         <v>168</v>
       </c>
@@ -13446,7 +13452,7 @@
         <v>Server</v>
       </c>
     </row>
-    <row r="172" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="7">
         <v>171</v>
       </c>
@@ -13521,7 +13527,7 @@
         <v>Server</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="7">
         <v>173</v>
       </c>
@@ -14721,7 +14727,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="203" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="7">
         <v>202</v>
       </c>
@@ -14880,7 +14886,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="207" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="7">
         <v>206</v>
       </c>
@@ -14922,7 +14928,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="208" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="7">
         <v>207</v>
       </c>
@@ -14964,7 +14970,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="209" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="7">
         <v>208</v>
       </c>
@@ -15006,7 +15012,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="210" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="7">
         <v>209</v>
       </c>
@@ -15048,7 +15054,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="211" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="7">
         <v>210</v>
       </c>
@@ -15090,7 +15096,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="212" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="7">
         <v>211</v>
       </c>
@@ -15132,7 +15138,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="213" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="7">
         <v>212</v>
       </c>
@@ -15174,7 +15180,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="214" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="7">
         <v>213</v>
       </c>
@@ -15216,7 +15222,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="215" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="7">
         <v>214</v>
       </c>
@@ -15258,7 +15264,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="216" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="7">
         <v>215</v>
       </c>
@@ -15300,7 +15306,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="217" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="7">
         <v>216</v>
       </c>
@@ -15459,7 +15465,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="221" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="7">
         <v>220</v>
       </c>
@@ -15501,7 +15507,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="222" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="7">
         <v>221</v>
       </c>
@@ -15582,7 +15588,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="224" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="7">
         <v>223</v>
       </c>
@@ -15624,7 +15630,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="225" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="7">
         <v>224</v>
       </c>
@@ -15872,7 +15878,7 @@
         <v>support-requirements</v>
       </c>
     </row>
-    <row r="232" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="7">
         <v>231</v>
       </c>
@@ -15992,7 +15998,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="235" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="7">
         <v>234</v>
       </c>
@@ -16040,7 +16046,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="236" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="7">
         <v>235</v>
       </c>
@@ -16085,7 +16091,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="237" spans="1:23" ht="153" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:23" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="7">
         <v>236</v>
       </c>
@@ -16127,7 +16133,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="238" spans="1:23" ht="153" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:23" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="7">
         <v>237</v>
       </c>
@@ -16169,7 +16175,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="239" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="7">
         <v>238</v>
       </c>
@@ -16203,7 +16209,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="240" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="7">
         <v>239</v>
       </c>
@@ -16237,7 +16243,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="241" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="7">
         <v>240</v>
       </c>
@@ -16271,7 +16277,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="242" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="7">
         <v>241</v>
       </c>
@@ -16468,7 +16474,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="248" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="7">
         <v>247</v>
       </c>
@@ -16591,7 +16597,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="251" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="7">
         <v>250</v>
       </c>
@@ -16675,7 +16681,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="253" spans="1:23" ht="221" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:23" ht="221" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="7">
         <v>252</v>
       </c>
@@ -16720,7 +16726,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="254" spans="1:23" ht="221" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:23" ht="221" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="7">
         <v>253</v>
       </c>
@@ -16765,7 +16771,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="255" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="7">
         <v>254</v>
       </c>
@@ -16852,7 +16858,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="257" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="7">
         <v>256</v>
       </c>
@@ -17269,7 +17275,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="267" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:23" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="7">
         <v>266</v>
       </c>
@@ -17389,7 +17395,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="270" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="7">
         <v>269</v>
       </c>
@@ -17560,7 +17566,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="274" spans="1:23" ht="153" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:23" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="7">
         <v>273</v>
       </c>
@@ -17602,7 +17608,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="275" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="7">
         <v>274</v>
       </c>
@@ -18607,7 +18613,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="301" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" s="7">
         <v>300</v>
       </c>
@@ -18688,7 +18694,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="303" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" s="7">
         <v>302</v>
       </c>
@@ -18730,7 +18736,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="304" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" s="7">
         <v>303</v>
       </c>
@@ -18772,7 +18778,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="305" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:23" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" s="7">
         <v>304</v>
       </c>
@@ -18853,7 +18859,7 @@
         <v/>
       </c>
     </row>
-    <row r="307" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" s="7">
         <v>306</v>
       </c>
@@ -18895,7 +18901,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="308" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" s="7">
         <v>307</v>
       </c>
@@ -19132,7 +19138,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="314" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" s="7">
         <v>313</v>
       </c>
@@ -19321,7 +19327,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="319" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" s="7">
         <v>318</v>
       </c>
@@ -19360,7 +19366,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="320" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" s="7">
         <v>319</v>
       </c>
@@ -19438,7 +19444,7 @@
         <v/>
       </c>
     </row>
-    <row r="322" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" s="7">
         <v>321</v>
       </c>
@@ -20242,7 +20248,7 @@
         <v/>
       </c>
     </row>
-    <row r="343" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" s="7">
         <v>342</v>
       </c>
@@ -20281,7 +20287,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="344" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" s="7">
         <v>343</v>
       </c>
@@ -20758,7 +20764,7 @@
         <v/>
       </c>
     </row>
-    <row r="357" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357" s="7">
         <v>356</v>
       </c>
@@ -20800,7 +20806,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="358" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358" s="7">
         <v>357</v>
       </c>
@@ -20920,7 +20926,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="361" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361" s="7">
         <v>360</v>
       </c>
@@ -21112,7 +21118,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="366" spans="1:23" ht="221" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:23" ht="221" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" s="7">
         <v>365</v>
       </c>
@@ -21226,7 +21232,7 @@
         <v/>
       </c>
     </row>
-    <row r="369" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" s="7">
         <v>368</v>
       </c>
@@ -21379,7 +21385,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="373" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373" s="7">
         <v>372</v>
       </c>
@@ -21418,7 +21424,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="374" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" s="7">
         <v>373</v>
       </c>
@@ -21457,7 +21463,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="375" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" s="7">
         <v>374</v>
       </c>
@@ -21496,7 +21502,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="376" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" s="7">
         <v>375</v>
       </c>
@@ -21652,7 +21658,7 @@
         <v/>
       </c>
     </row>
-    <row r="380" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380" s="7">
         <v>379</v>
       </c>
@@ -21766,7 +21772,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="383" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383" s="7">
         <v>382</v>
       </c>
@@ -21808,7 +21814,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="384" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384" s="7">
         <v>383</v>
       </c>
@@ -21967,7 +21973,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="388" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388" s="7">
         <v>387</v>
       </c>
@@ -22078,7 +22084,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="391" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391" s="7">
         <v>390</v>
       </c>
@@ -22117,7 +22123,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="392" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392" s="7">
         <v>391</v>
       </c>
@@ -22345,7 +22351,7 @@
         <v/>
       </c>
     </row>
-    <row r="398" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398" s="7">
         <v>397</v>
       </c>
@@ -22498,7 +22504,7 @@
         <v/>
       </c>
     </row>
-    <row r="402" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402" s="7">
         <v>401</v>
       </c>
@@ -22540,7 +22546,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="403" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403" s="7">
         <v>402</v>
       </c>
@@ -22654,7 +22660,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="406" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" s="7">
         <v>405</v>
       </c>
@@ -22699,7 +22705,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="407" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407" s="7">
         <v>406</v>
       </c>
@@ -22780,7 +22786,7 @@
         <v/>
       </c>
     </row>
-    <row r="409" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409" s="7">
         <v>408</v>
       </c>
@@ -22894,7 +22900,7 @@
         <v>Client</v>
       </c>
     </row>
-    <row r="412" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412" s="7">
         <v>411</v>
       </c>
@@ -23023,7 +23029,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="415" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415" s="7">
         <v>414</v>
       </c>
@@ -23305,7 +23311,7 @@
         <v/>
       </c>
     </row>
-    <row r="422" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422" s="7">
         <v>421</v>
       </c>
@@ -23464,7 +23470,7 @@
         <v/>
       </c>
     </row>
-    <row r="426" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426" s="7">
         <v>425</v>
       </c>
@@ -23545,7 +23551,7 @@
         <v/>
       </c>
     </row>
-    <row r="428" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A428" s="7">
         <v>427</v>
       </c>
@@ -23743,7 +23749,7 @@
         <v/>
       </c>
     </row>
-    <row r="433" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A433" s="7">
         <v>432</v>
       </c>
@@ -23785,7 +23791,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="434" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A434" s="7">
         <v>433</v>
       </c>
@@ -23824,7 +23830,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="435" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A435" s="7">
         <v>434</v>
       </c>
@@ -23863,7 +23869,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="436" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A436" s="7">
         <v>435</v>
       </c>
@@ -23902,7 +23908,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="437" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A437" s="7">
         <v>436</v>
       </c>
@@ -24019,7 +24025,7 @@
         <v/>
       </c>
     </row>
-    <row r="440" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:23" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A440" s="7">
         <v>439</v>
       </c>
@@ -24211,7 +24217,7 @@
         <v/>
       </c>
     </row>
-    <row r="445" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A445" s="7">
         <v>444</v>
       </c>
@@ -24442,7 +24448,7 @@
         <v/>
       </c>
     </row>
-    <row r="451" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" s="7">
         <v>450</v>
       </c>
@@ -24484,7 +24490,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="452" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" s="7">
         <v>451</v>
       </c>
@@ -24643,7 +24649,7 @@
         <v/>
       </c>
     </row>
-    <row r="456" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A456" s="7">
         <v>455</v>
       </c>
@@ -24790,7 +24796,7 @@
         <v/>
       </c>
     </row>
-    <row r="460" spans="1:23" ht="187" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:23" ht="187" hidden="1" x14ac:dyDescent="0.2">
       <c r="A460" s="7">
         <v>459</v>
       </c>
@@ -24835,7 +24841,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="461" spans="1:23" ht="187" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:23" ht="187" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461" s="7">
         <v>460</v>
       </c>
@@ -24964,7 +24970,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="464" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A464" s="7">
         <v>463</v>
       </c>
@@ -25009,7 +25015,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="465" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:23" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A465" s="7">
         <v>464</v>
       </c>
@@ -25054,7 +25060,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="466" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A466" s="7">
         <v>465</v>
       </c>
@@ -25205,7 +25211,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="470" spans="1:23" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:23" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A470" s="7">
         <v>469</v>
       </c>
@@ -25364,7 +25370,7 @@
         <v/>
       </c>
     </row>
-    <row r="474" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A474" s="7">
         <v>473</v>
       </c>
@@ -25445,7 +25451,7 @@
         <v>Server</v>
       </c>
     </row>
-    <row r="476" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A476" s="7">
         <v>475</v>
       </c>
@@ -25703,7 +25709,7 @@
         <v/>
       </c>
     </row>
-    <row r="483" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A483" s="7">
         <v>482</v>
       </c>
@@ -25790,7 +25796,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="485" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:23" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A485" s="7">
         <v>484</v>
       </c>
@@ -25877,7 +25883,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="487" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A487" s="7">
         <v>486</v>
       </c>
@@ -26006,7 +26012,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="490" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A490" s="7">
         <v>489</v>
       </c>
@@ -26045,7 +26051,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="491" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A491" s="7">
         <v>490</v>
       </c>
@@ -26084,7 +26090,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="492" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A492" s="7">
         <v>491</v>
       </c>
@@ -26123,7 +26129,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="493" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A493" s="7">
         <v>492</v>
       </c>
@@ -26162,7 +26168,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="494" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A494" s="7">
         <v>493</v>
       </c>
@@ -26201,7 +26207,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="495" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A495" s="7">
         <v>494</v>
       </c>
@@ -26240,7 +26246,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="496" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A496" s="7">
         <v>495</v>
       </c>
@@ -26279,7 +26285,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="497" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A497" s="7">
         <v>496</v>
       </c>
@@ -26318,7 +26324,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="498" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A498" s="7">
         <v>497</v>
       </c>
@@ -26357,7 +26363,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="499" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A499" s="7">
         <v>498</v>
       </c>
@@ -26396,7 +26402,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="500" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A500" s="7">
         <v>499</v>
       </c>
@@ -26435,7 +26441,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="501" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A501" s="7">
         <v>500</v>
       </c>
@@ -26474,7 +26480,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="502" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A502" s="7">
         <v>501</v>
       </c>
@@ -26513,7 +26519,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="503" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A503" s="7">
         <v>502</v>
       </c>
@@ -26552,7 +26558,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="504" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A504" s="7">
         <v>503</v>
       </c>
@@ -26591,7 +26597,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="505" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A505" s="7">
         <v>504</v>
       </c>
@@ -26630,7 +26636,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="506" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A506" s="7">
         <v>505</v>
       </c>
@@ -26669,7 +26675,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="507" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A507" s="7">
         <v>506</v>
       </c>
@@ -26708,7 +26714,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="508" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A508" s="7">
         <v>507</v>
       </c>
@@ -26747,7 +26753,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="509" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A509" s="7">
         <v>508</v>
       </c>
@@ -26867,7 +26873,7 @@
         <v/>
       </c>
     </row>
-    <row r="512" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A512" s="7">
         <v>511</v>
       </c>
@@ -27062,7 +27068,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="517" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A517" s="7">
         <v>516</v>
       </c>
@@ -27149,7 +27155,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="519" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:23" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A519" s="7">
         <v>518</v>
       </c>
@@ -27236,7 +27242,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="521" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:23" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A521" s="7">
         <v>520</v>
       </c>
@@ -27401,7 +27407,7 @@
         <v/>
       </c>
     </row>
-    <row r="525" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:23" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A525" s="7">
         <v>524</v>
       </c>
@@ -27737,7 +27743,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="534" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A534" s="7">
         <v>533</v>
       </c>
@@ -27776,7 +27782,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="535" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A535" s="7">
         <v>534</v>
       </c>
@@ -27807,7 +27813,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="536" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A536" s="7">
         <v>535</v>
       </c>
@@ -27838,7 +27844,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="537" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A537" s="7">
         <v>536</v>
       </c>
@@ -27869,7 +27875,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="538" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A538" s="7">
         <v>537</v>
       </c>
@@ -27900,7 +27906,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="539" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A539" s="7">
         <v>538</v>
       </c>
@@ -27931,7 +27937,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="540" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A540" s="7">
         <v>539</v>
       </c>
@@ -27962,7 +27968,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="541" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A541" s="7">
         <v>540</v>
       </c>
@@ -28049,7 +28055,7 @@
         <v>behavior</v>
       </c>
     </row>
-    <row r="544" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A544" s="7">
         <v>543</v>
       </c>
@@ -28254,7 +28260,7 @@
         <v>valueset</v>
       </c>
     </row>
-    <row r="551" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A551" s="7">
         <v>550</v>
       </c>
@@ -28481,7 +28487,7 @@
         <v>patient-privacy-and-security</v>
       </c>
     </row>
-    <row r="559" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A559" s="7">
         <v>558</v>
       </c>
@@ -28596,7 +28602,7 @@
         <v>patient-privacy-and-security</v>
       </c>
     </row>
-    <row r="563" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:23" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A563" s="7">
         <v>562</v>
       </c>
@@ -28655,7 +28661,7 @@
         <v>patient-privacy-and-security</v>
       </c>
     </row>
-    <row r="565" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A565" s="7">
         <v>564</v>
       </c>
@@ -28770,7 +28776,7 @@
         <v>patient-privacy-and-security</v>
       </c>
     </row>
-    <row r="569" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A569" s="7">
         <v>568</v>
       </c>
@@ -28829,7 +28835,7 @@
         <v>patient-privacy-and-security</v>
       </c>
     </row>
-    <row r="571" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:23" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A571" s="7">
         <v>570</v>
       </c>
@@ -28891,7 +28897,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="573" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:23" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A573" s="7">
         <v>572</v>
       </c>
@@ -29205,7 +29211,7 @@
         <v>current-binding-for-coded-elements</v>
       </c>
     </row>
-    <row r="584" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="584" spans="1:24" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A584" s="7">
         <v>583</v>
       </c>
@@ -29239,7 +29245,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="585" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:24" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A585" s="7">
         <v>584</v>
       </c>
@@ -29301,7 +29307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="587" spans="1:24" ht="153" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:24" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A587" s="7">
         <v>801</v>
       </c>
@@ -29333,7 +29339,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="588" spans="1:24" ht="102" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:24" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A588" s="7">
         <v>802</v>
       </c>
@@ -29365,7 +29371,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="589" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:24" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A589" s="7">
         <v>803</v>
       </c>
@@ -29394,7 +29400,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="590" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:24" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A590" s="7">
         <v>804</v>
       </c>
@@ -29426,7 +29432,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="591" spans="1:24" ht="85" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:24" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A591" s="7">
         <v>805</v>
       </c>
@@ -29485,7 +29491,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="593" spans="1:24" ht="85" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:24" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A593" s="7">
         <v>809</v>
       </c>
@@ -29546,7 +29552,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="595" spans="1:24" ht="119" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:24" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A595" s="7">
         <v>811</v>
       </c>
@@ -29578,7 +29584,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="596" spans="1:24" ht="85" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:24" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A596" s="7">
         <v>812</v>
       </c>
@@ -29636,7 +29642,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="598" spans="1:24" ht="85" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:24" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A598" s="7">
         <v>814</v>
       </c>
@@ -29737,7 +29743,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="602" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:24" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A602" s="7">
         <v>818</v>
       </c>
@@ -29763,7 +29769,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="603" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:24" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A603" s="7">
         <v>819</v>
       </c>
@@ -29841,7 +29847,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="606" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:24" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A606" s="7">
         <v>822</v>
       </c>
@@ -29867,7 +29873,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="607" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="607" spans="1:24" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A607" s="7">
         <v>823</v>
       </c>
@@ -29893,7 +29899,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="608" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:24" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A608" s="7">
         <v>824</v>
       </c>
@@ -29959,7 +29965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="611" spans="1:24" ht="238" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:24" ht="238" hidden="1" x14ac:dyDescent="0.2">
       <c r="A611" s="7">
         <v>827</v>
       </c>
@@ -30045,7 +30051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="615" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="615" spans="1:24" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A615" s="7">
         <v>831</v>
       </c>
@@ -30071,7 +30077,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="616" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="616" spans="1:24" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A616" s="7">
         <v>832</v>
       </c>
@@ -30097,7 +30103,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="617" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:24" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A617" s="7">
         <v>833</v>
       </c>
@@ -30255,7 +30261,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="624" spans="1:24" ht="85" x14ac:dyDescent="0.2">
+    <row r="624" spans="1:24" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A624" s="7">
         <v>840</v>
       </c>
@@ -30376,7 +30382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="629" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="629" spans="1:24" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A629" s="7">
         <v>845</v>
       </c>
@@ -30402,7 +30408,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="630" spans="1:24" ht="85" x14ac:dyDescent="0.2">
+    <row r="630" spans="1:24" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A630" s="7">
         <v>846</v>
       </c>
@@ -30534,7 +30540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="636" spans="1:24" ht="119" x14ac:dyDescent="0.2">
+    <row r="636" spans="1:24" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A636" s="7">
         <v>852</v>
       </c>
@@ -30764,7 +30770,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="646" spans="1:24" ht="119" x14ac:dyDescent="0.2">
+    <row r="646" spans="1:24" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A646" s="7">
         <v>862</v>
       </c>
@@ -30838,6 +30844,15 @@
       <c r="G648" s="7" t="b">
         <v>0</v>
       </c>
+      <c r="K648" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="L648" s="22" t="s">
+        <v>1160</v>
+      </c>
+      <c r="V648" s="12" t="s">
+        <v>1159</v>
+      </c>
       <c r="W648" s="6" t="s">
         <v>1141</v>
       </c>
@@ -30868,7 +30883,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="650" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="650" spans="1:24" ht="68" x14ac:dyDescent="0.2">
       <c r="A650" s="7">
         <v>866</v>
       </c>
@@ -30886,6 +30901,15 @@
       </c>
       <c r="G650" s="7" t="b">
         <v>0</v>
+      </c>
+      <c r="K650" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="L650" s="22" t="s">
+        <v>1160</v>
+      </c>
+      <c r="V650" s="12" t="s">
+        <v>1159</v>
       </c>
       <c r="W650" s="6" t="s">
         <v>1141</v>
@@ -30917,7 +30941,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="652" spans="1:24" ht="119" x14ac:dyDescent="0.2">
+    <row r="652" spans="1:24" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A652" s="7">
         <v>868</v>
       </c>
@@ -30963,7 +30987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="654" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="654" spans="1:24" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A654" s="7">
         <v>870</v>
       </c>
@@ -31015,7 +31039,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="656" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="656" spans="1:24" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A656" s="7">
         <v>872</v>
       </c>
@@ -31045,16 +31069,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W656" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
-    <filterColumn colId="3">
+  <autoFilter ref="A1:X656" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
+    <filterColumn colId="22">
       <filters>
-        <filter val="SHALL"/>
-        <filter val="SHALL NOT"/>
+        <filter val="y"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="4">
+    <filterColumn colId="23">
       <filters>
-        <filter val="Server"/>
+        <filter val="?"/>
+        <filter val="validation?"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>